<commit_message>
Added Named Ranges to Companies spreadsheets.
</commit_message>
<xml_diff>
--- a/src/LinqToExcel.Tests/ExcelFiles/Companies.xlsx
+++ b/src/LinqToExcel.Tests/ExcelFiles/Companies.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="45" windowWidth="15315" windowHeight="13575" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="360" yWindow="45" windowWidth="15315" windowHeight="13575" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,6 +16,9 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">AutoFiltered!$A$1:$D$8</definedName>
+    <definedName name="Companies">Sheet1!$A$1:$D$8</definedName>
+    <definedName name="MoreCompanies">MoreCompanies!$A$1:$D$4</definedName>
+    <definedName name="NullCellCompanies">NullCells!$A$1:$D$4</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="3">AutoFiltered!$A$1:$B$6</definedName>
     <definedName name="Range1">'Paul''s Worksheet'!$A$1:$D$11</definedName>
     <definedName name="Range2">'Paul''s Worksheet'!$A$1:$D$11</definedName>
@@ -473,7 +476,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D4"/>
+      <selection activeCell="D8" sqref="A1:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -842,7 +845,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="D4" sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1054,8 +1057,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1125,7 +1128,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5:H16"/>
     </sheetView>
   </sheetViews>

</xml_diff>